<commit_message>
nuevos datos en simulacion y nuevo archivo con actualizacciones
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2756"/>
+  <dimension ref="A1:F2843"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42531,6 +42531,1526 @@
         <v>50</v>
       </c>
     </row>
+    <row r="2757">
+      <c r="A2757" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2757" t="inlineStr">
+        <is>
+          <t>[1, 3, 19]</t>
+        </is>
+      </c>
+      <c r="C2757" t="inlineStr"/>
+      <c r="D2757" t="inlineStr"/>
+      <c r="E2757" t="inlineStr"/>
+      <c r="F2757" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2758">
+      <c r="A2758" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2758" t="inlineStr">
+        <is>
+          <t>[3, 9, 14]</t>
+        </is>
+      </c>
+      <c r="C2758" t="inlineStr"/>
+      <c r="D2758" t="inlineStr"/>
+      <c r="E2758" t="inlineStr"/>
+      <c r="F2758" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2759">
+      <c r="A2759" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2759" t="inlineStr">
+        <is>
+          <t>[3, 8, 14]</t>
+        </is>
+      </c>
+      <c r="C2759" t="inlineStr"/>
+      <c r="D2759" t="inlineStr"/>
+      <c r="E2759" t="inlineStr"/>
+      <c r="F2759" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2760">
+      <c r="A2760" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2760" t="inlineStr">
+        <is>
+          <t>[3, 7, 14]</t>
+        </is>
+      </c>
+      <c r="C2760" t="inlineStr"/>
+      <c r="D2760" t="inlineStr"/>
+      <c r="E2760" t="inlineStr"/>
+      <c r="F2760" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2761">
+      <c r="A2761" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2761" t="inlineStr">
+        <is>
+          <t>[2, 12, 13]</t>
+        </is>
+      </c>
+      <c r="C2761" t="inlineStr"/>
+      <c r="D2761" t="inlineStr"/>
+      <c r="E2761" t="inlineStr"/>
+      <c r="F2761" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2762">
+      <c r="A2762" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2762" t="inlineStr">
+        <is>
+          <t>[6, 17, 22]</t>
+        </is>
+      </c>
+      <c r="C2762" t="inlineStr"/>
+      <c r="D2762" t="inlineStr"/>
+      <c r="E2762" t="inlineStr"/>
+      <c r="F2762" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2763">
+      <c r="A2763" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2763" t="inlineStr">
+        <is>
+          <t>[14, 17, 34]</t>
+        </is>
+      </c>
+      <c r="C2763" t="inlineStr"/>
+      <c r="D2763" t="inlineStr"/>
+      <c r="E2763" t="inlineStr"/>
+      <c r="F2763" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2764">
+      <c r="A2764" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2764" t="inlineStr">
+        <is>
+          <t>[5, 18, 34]</t>
+        </is>
+      </c>
+      <c r="C2764" t="inlineStr"/>
+      <c r="D2764" t="inlineStr"/>
+      <c r="E2764" t="inlineStr"/>
+      <c r="F2764" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2765">
+      <c r="A2765" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2765" t="inlineStr">
+        <is>
+          <t>[18, 32, 34]</t>
+        </is>
+      </c>
+      <c r="C2765" t="inlineStr"/>
+      <c r="D2765" t="inlineStr"/>
+      <c r="E2765" t="inlineStr"/>
+      <c r="F2765" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2766">
+      <c r="A2766" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2766" t="inlineStr">
+        <is>
+          <t>[16, 28, 34]</t>
+        </is>
+      </c>
+      <c r="C2766" t="inlineStr"/>
+      <c r="D2766" t="inlineStr"/>
+      <c r="E2766" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2766" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2767">
+      <c r="A2767" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2767" t="inlineStr">
+        <is>
+          <t>[16, 28, 32]</t>
+        </is>
+      </c>
+      <c r="C2767" t="inlineStr"/>
+      <c r="D2767" t="inlineStr"/>
+      <c r="E2767" t="inlineStr"/>
+      <c r="F2767" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2768">
+      <c r="A2768" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2768" t="inlineStr">
+        <is>
+          <t>[12, 16, 32]</t>
+        </is>
+      </c>
+      <c r="C2768" t="inlineStr"/>
+      <c r="D2768" t="inlineStr"/>
+      <c r="E2768" t="inlineStr"/>
+      <c r="F2768" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2769">
+      <c r="A2769" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2769" t="inlineStr">
+        <is>
+          <t>[18, 27, 32]</t>
+        </is>
+      </c>
+      <c r="C2769" t="inlineStr"/>
+      <c r="D2769" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2769" t="inlineStr"/>
+      <c r="F2769" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2770">
+      <c r="A2770" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2770" t="inlineStr">
+        <is>
+          <t>[4, 23, 25]</t>
+        </is>
+      </c>
+      <c r="C2770" t="inlineStr"/>
+      <c r="D2770" t="inlineStr"/>
+      <c r="E2770" t="inlineStr"/>
+      <c r="F2770" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2771">
+      <c r="A2771" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2771" t="inlineStr">
+        <is>
+          <t>[4, 23, 31]</t>
+        </is>
+      </c>
+      <c r="C2771" t="inlineStr"/>
+      <c r="D2771" t="inlineStr"/>
+      <c r="E2771" t="inlineStr"/>
+      <c r="F2771" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2772">
+      <c r="A2772" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2772" t="inlineStr">
+        <is>
+          <t>[5, 28, 29]</t>
+        </is>
+      </c>
+      <c r="C2772" t="inlineStr"/>
+      <c r="D2772" t="inlineStr"/>
+      <c r="E2772" t="inlineStr"/>
+      <c r="F2772" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2773">
+      <c r="A2773" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2773" t="inlineStr">
+        <is>
+          <t>[14, 26, 36]</t>
+        </is>
+      </c>
+      <c r="C2773" t="inlineStr"/>
+      <c r="D2773" t="inlineStr"/>
+      <c r="E2773" t="inlineStr"/>
+      <c r="F2773" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2774">
+      <c r="A2774" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2774" t="inlineStr">
+        <is>
+          <t>[10, 14, 26]</t>
+        </is>
+      </c>
+      <c r="C2774" t="inlineStr"/>
+      <c r="D2774" t="inlineStr"/>
+      <c r="E2774" t="inlineStr"/>
+      <c r="F2774" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2775">
+      <c r="A2775" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2775" t="inlineStr">
+        <is>
+          <t>[20, 25, 28]</t>
+        </is>
+      </c>
+      <c r="C2775" t="inlineStr"/>
+      <c r="D2775" t="inlineStr"/>
+      <c r="E2775" t="inlineStr"/>
+      <c r="F2775" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2776">
+      <c r="A2776" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2776" t="inlineStr">
+        <is>
+          <t>[1, 20, 34]</t>
+        </is>
+      </c>
+      <c r="C2776" t="inlineStr"/>
+      <c r="D2776" t="inlineStr"/>
+      <c r="E2776" t="inlineStr"/>
+      <c r="F2776" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2777">
+      <c r="A2777" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2777" t="inlineStr">
+        <is>
+          <t>[1, 27, 34]</t>
+        </is>
+      </c>
+      <c r="C2777" t="inlineStr"/>
+      <c r="D2777" t="inlineStr"/>
+      <c r="E2777" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2777" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2778">
+      <c r="A2778" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2778" t="inlineStr">
+        <is>
+          <t>[14, 24, 33]</t>
+        </is>
+      </c>
+      <c r="C2778" t="inlineStr"/>
+      <c r="D2778" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2778" t="inlineStr"/>
+      <c r="F2778" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2779">
+      <c r="A2779" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2779" t="inlineStr">
+        <is>
+          <t>[3, 12, 15]</t>
+        </is>
+      </c>
+      <c r="C2779" t="inlineStr"/>
+      <c r="D2779" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2779" t="inlineStr"/>
+      <c r="F2779" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2780">
+      <c r="A2780" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2780" t="inlineStr">
+        <is>
+          <t>[12, 24, 30]</t>
+        </is>
+      </c>
+      <c r="C2780" t="inlineStr"/>
+      <c r="D2780" t="inlineStr"/>
+      <c r="E2780" t="inlineStr"/>
+      <c r="F2780" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2781">
+      <c r="A2781" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2781" t="inlineStr">
+        <is>
+          <t>[15, 17, 30]</t>
+        </is>
+      </c>
+      <c r="C2781" t="inlineStr"/>
+      <c r="D2781" t="inlineStr"/>
+      <c r="E2781" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2781" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2782">
+      <c r="A2782" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2782" t="inlineStr">
+        <is>
+          <t>[14, 15, 24]</t>
+        </is>
+      </c>
+      <c r="C2782" t="inlineStr"/>
+      <c r="D2782" t="inlineStr"/>
+      <c r="E2782" t="inlineStr"/>
+      <c r="F2782" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2783">
+      <c r="A2783" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2783" t="inlineStr">
+        <is>
+          <t>[15, 18, 34]</t>
+        </is>
+      </c>
+      <c r="C2783" t="inlineStr"/>
+      <c r="D2783" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2783" t="inlineStr"/>
+      <c r="F2783" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2784">
+      <c r="A2784" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2784" t="inlineStr">
+        <is>
+          <t>[15, 32, 34]</t>
+        </is>
+      </c>
+      <c r="C2784" t="inlineStr"/>
+      <c r="D2784" t="inlineStr"/>
+      <c r="E2784" t="inlineStr"/>
+      <c r="F2784" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2785">
+      <c r="A2785" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2785" t="inlineStr">
+        <is>
+          <t>[16, 19, 28]</t>
+        </is>
+      </c>
+      <c r="C2785" t="inlineStr"/>
+      <c r="D2785" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2785" t="inlineStr"/>
+      <c r="F2785" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2786">
+      <c r="A2786" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2786" t="inlineStr">
+        <is>
+          <t>[12, 18, 28]</t>
+        </is>
+      </c>
+      <c r="C2786" t="inlineStr"/>
+      <c r="D2786" t="inlineStr"/>
+      <c r="E2786" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2786" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2787">
+      <c r="A2787" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2787" t="inlineStr">
+        <is>
+          <t>[12, 20, 35]</t>
+        </is>
+      </c>
+      <c r="C2787" t="inlineStr"/>
+      <c r="D2787" t="inlineStr"/>
+      <c r="E2787" t="inlineStr"/>
+      <c r="F2787" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2788">
+      <c r="A2788" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2788" t="inlineStr">
+        <is>
+          <t>[7, 19, 34]</t>
+        </is>
+      </c>
+      <c r="C2788" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2788" t="inlineStr"/>
+      <c r="E2788" t="inlineStr"/>
+      <c r="F2788" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2789">
+      <c r="A2789" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2789" t="inlineStr">
+        <is>
+          <t>[7, 27, 32]</t>
+        </is>
+      </c>
+      <c r="C2789" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2789" t="inlineStr"/>
+      <c r="E2789" t="inlineStr"/>
+      <c r="F2789" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2790">
+      <c r="A2790" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2790" t="inlineStr">
+        <is>
+          <t>[0, 20, 31]</t>
+        </is>
+      </c>
+      <c r="C2790" t="inlineStr"/>
+      <c r="D2790" t="inlineStr"/>
+      <c r="E2790" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2790" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2791">
+      <c r="A2791" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2791" t="inlineStr">
+        <is>
+          <t>[0, 3, 32]</t>
+        </is>
+      </c>
+      <c r="C2791" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2791" t="inlineStr"/>
+      <c r="E2791" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2791" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2792">
+      <c r="A2792" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2792" t="inlineStr">
+        <is>
+          <t>[0, 6, 17]</t>
+        </is>
+      </c>
+      <c r="C2792" t="inlineStr"/>
+      <c r="D2792" t="inlineStr"/>
+      <c r="E2792" t="inlineStr"/>
+      <c r="F2792" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2793">
+      <c r="A2793" t="n">
+        <v>18</v>
+      </c>
+      <c r="B2793" t="inlineStr">
+        <is>
+          <t>[6, 17, 32]</t>
+        </is>
+      </c>
+      <c r="C2793" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2793" t="inlineStr"/>
+      <c r="E2793" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2793" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2794">
+      <c r="A2794" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2794" t="inlineStr">
+        <is>
+          <t>[15, 17, 34]</t>
+        </is>
+      </c>
+      <c r="C2794" t="inlineStr"/>
+      <c r="D2794" t="inlineStr"/>
+      <c r="E2794" t="inlineStr"/>
+      <c r="F2794" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2795">
+      <c r="A2795" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2795" t="inlineStr">
+        <is>
+          <t>[0, 22, 36]</t>
+        </is>
+      </c>
+      <c r="C2795" t="inlineStr"/>
+      <c r="D2795" t="inlineStr"/>
+      <c r="E2795" t="inlineStr"/>
+      <c r="F2795" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2796">
+      <c r="A2796" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2796" t="inlineStr">
+        <is>
+          <t>[11, 17, 22]</t>
+        </is>
+      </c>
+      <c r="C2796" t="inlineStr"/>
+      <c r="D2796" t="inlineStr"/>
+      <c r="E2796" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2796" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2797">
+      <c r="A2797" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2797" t="inlineStr">
+        <is>
+          <t>[7, 25, 34]</t>
+        </is>
+      </c>
+      <c r="C2797" t="inlineStr"/>
+      <c r="D2797" t="inlineStr"/>
+      <c r="E2797" t="inlineStr"/>
+      <c r="F2797" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2798">
+      <c r="A2798" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2798" t="inlineStr">
+        <is>
+          <t>[7, 13, 16]</t>
+        </is>
+      </c>
+      <c r="C2798" t="inlineStr"/>
+      <c r="D2798" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2798" t="inlineStr"/>
+      <c r="F2798" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2799">
+      <c r="A2799" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2799" t="inlineStr">
+        <is>
+          <t>[18, 24, 26]</t>
+        </is>
+      </c>
+      <c r="C2799" t="inlineStr"/>
+      <c r="D2799" t="inlineStr"/>
+      <c r="E2799" t="inlineStr"/>
+      <c r="F2799" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2800">
+      <c r="A2800" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2800" t="inlineStr">
+        <is>
+          <t>[0, 16, 23]</t>
+        </is>
+      </c>
+      <c r="C2800" t="inlineStr"/>
+      <c r="D2800" t="inlineStr"/>
+      <c r="E2800" t="inlineStr"/>
+      <c r="F2800" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2801">
+      <c r="A2801" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2801" t="inlineStr">
+        <is>
+          <t>[22, 25, 26]</t>
+        </is>
+      </c>
+      <c r="C2801" t="inlineStr"/>
+      <c r="D2801" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2801" t="inlineStr"/>
+      <c r="F2801" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2802">
+      <c r="A2802" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2802" t="inlineStr">
+        <is>
+          <t>[3, 6, 33]</t>
+        </is>
+      </c>
+      <c r="C2802" t="inlineStr"/>
+      <c r="D2802" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2802" t="inlineStr"/>
+      <c r="F2802" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2803">
+      <c r="A2803" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2803" t="inlineStr">
+        <is>
+          <t>[2, 3, 4]</t>
+        </is>
+      </c>
+      <c r="C2803" t="inlineStr"/>
+      <c r="D2803" t="inlineStr"/>
+      <c r="E2803" t="inlineStr"/>
+      <c r="F2803" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2804">
+      <c r="A2804" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2804" t="inlineStr">
+        <is>
+          <t>[0, 10, 12]</t>
+        </is>
+      </c>
+      <c r="C2804" t="inlineStr"/>
+      <c r="D2804" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2804" t="inlineStr"/>
+      <c r="F2804" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2805">
+      <c r="A2805" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2805" t="inlineStr">
+        <is>
+          <t>[10, 12, 29]</t>
+        </is>
+      </c>
+      <c r="C2805" t="inlineStr"/>
+      <c r="D2805" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2805" t="inlineStr"/>
+      <c r="F2805" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2806">
+      <c r="A2806" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2806" t="inlineStr">
+        <is>
+          <t>[2, 10, 24]</t>
+        </is>
+      </c>
+      <c r="C2806" t="inlineStr"/>
+      <c r="D2806" t="inlineStr"/>
+      <c r="E2806" t="inlineStr"/>
+      <c r="F2806" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2807">
+      <c r="A2807" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2807" t="inlineStr">
+        <is>
+          <t>[10, 19, 24]</t>
+        </is>
+      </c>
+      <c r="C2807" t="inlineStr"/>
+      <c r="D2807" t="inlineStr"/>
+      <c r="E2807" t="inlineStr"/>
+      <c r="F2807" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2808">
+      <c r="A2808" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2808" t="inlineStr">
+        <is>
+          <t>[10, 28, 30]</t>
+        </is>
+      </c>
+      <c r="C2808" t="inlineStr"/>
+      <c r="D2808" t="inlineStr"/>
+      <c r="E2808" t="inlineStr"/>
+      <c r="F2808" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2809">
+      <c r="A2809" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2809" t="inlineStr">
+        <is>
+          <t>[10, 15, 21]</t>
+        </is>
+      </c>
+      <c r="C2809" t="inlineStr"/>
+      <c r="D2809" t="inlineStr"/>
+      <c r="E2809" t="inlineStr"/>
+      <c r="F2809" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2810">
+      <c r="A2810" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2810" t="inlineStr">
+        <is>
+          <t>[1, 13, 15]</t>
+        </is>
+      </c>
+      <c r="C2810" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2810" t="inlineStr"/>
+      <c r="E2810" t="inlineStr"/>
+      <c r="F2810" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2811">
+      <c r="A2811" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2811" t="inlineStr">
+        <is>
+          <t>[7, 14, 18]</t>
+        </is>
+      </c>
+      <c r="C2811" t="inlineStr"/>
+      <c r="D2811" t="inlineStr"/>
+      <c r="E2811" t="inlineStr"/>
+      <c r="F2811" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2812">
+      <c r="A2812" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2812" t="inlineStr">
+        <is>
+          <t>[9, 14, 18]</t>
+        </is>
+      </c>
+      <c r="C2812" t="inlineStr"/>
+      <c r="D2812" t="inlineStr"/>
+      <c r="E2812" t="inlineStr"/>
+      <c r="F2812" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2813">
+      <c r="A2813" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2813" t="inlineStr">
+        <is>
+          <t>[1, 14, 27]</t>
+        </is>
+      </c>
+      <c r="C2813" t="inlineStr"/>
+      <c r="D2813" t="inlineStr"/>
+      <c r="E2813" t="inlineStr"/>
+      <c r="F2813" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2814">
+      <c r="A2814" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2814" t="inlineStr">
+        <is>
+          <t>[1, 3, 36]</t>
+        </is>
+      </c>
+      <c r="C2814" t="inlineStr"/>
+      <c r="D2814" t="inlineStr"/>
+      <c r="E2814" t="inlineStr"/>
+      <c r="F2814" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2815">
+      <c r="A2815" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2815" t="inlineStr">
+        <is>
+          <t>[3, 24, 36]</t>
+        </is>
+      </c>
+      <c r="C2815" t="inlineStr"/>
+      <c r="D2815" t="inlineStr"/>
+      <c r="E2815" t="inlineStr"/>
+      <c r="F2815" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2816">
+      <c r="A2816" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2816" t="inlineStr">
+        <is>
+          <t>[2, 3, 12]</t>
+        </is>
+      </c>
+      <c r="C2816" t="inlineStr"/>
+      <c r="D2816" t="inlineStr"/>
+      <c r="E2816" t="inlineStr"/>
+      <c r="F2816" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2817">
+      <c r="A2817" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2817" t="inlineStr">
+        <is>
+          <t>[0, 11, 29]</t>
+        </is>
+      </c>
+      <c r="C2817" t="inlineStr"/>
+      <c r="D2817" t="inlineStr"/>
+      <c r="E2817" t="inlineStr"/>
+      <c r="F2817" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2818">
+      <c r="A2818" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2818" t="inlineStr">
+        <is>
+          <t>[3, 11, 21]</t>
+        </is>
+      </c>
+      <c r="C2818" t="inlineStr"/>
+      <c r="D2818" t="inlineStr"/>
+      <c r="E2818" t="inlineStr"/>
+      <c r="F2818" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2819">
+      <c r="A2819" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2819" t="inlineStr">
+        <is>
+          <t>[11, 20, 33]</t>
+        </is>
+      </c>
+      <c r="C2819" t="inlineStr"/>
+      <c r="D2819" t="inlineStr"/>
+      <c r="E2819" t="inlineStr"/>
+      <c r="F2819" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2820">
+      <c r="A2820" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2820" t="inlineStr">
+        <is>
+          <t>[25, 32, 34]</t>
+        </is>
+      </c>
+      <c r="C2820" t="inlineStr"/>
+      <c r="D2820" t="inlineStr"/>
+      <c r="E2820" t="inlineStr"/>
+      <c r="F2820" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2821">
+      <c r="A2821" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2821" t="inlineStr">
+        <is>
+          <t>[25, 28, 29]</t>
+        </is>
+      </c>
+      <c r="C2821" t="inlineStr"/>
+      <c r="D2821" t="inlineStr"/>
+      <c r="E2821" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2821" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2822">
+      <c r="A2822" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2822" t="inlineStr">
+        <is>
+          <t>[1, 12, 28]</t>
+        </is>
+      </c>
+      <c r="C2822" t="inlineStr"/>
+      <c r="D2822" t="inlineStr"/>
+      <c r="E2822" t="inlineStr"/>
+      <c r="F2822" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2823">
+      <c r="A2823" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2823" t="inlineStr">
+        <is>
+          <t>[6, 13, 35]</t>
+        </is>
+      </c>
+      <c r="C2823" t="inlineStr"/>
+      <c r="D2823" t="inlineStr"/>
+      <c r="E2823" t="inlineStr"/>
+      <c r="F2823" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2824">
+      <c r="A2824" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2824" t="inlineStr">
+        <is>
+          <t>[25, 32, 33]</t>
+        </is>
+      </c>
+      <c r="C2824" t="inlineStr"/>
+      <c r="D2824" t="inlineStr"/>
+      <c r="E2824" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2824" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2825">
+      <c r="A2825" t="n">
+        <v>21</v>
+      </c>
+      <c r="B2825" t="inlineStr">
+        <is>
+          <t>[11, 17, 25]</t>
+        </is>
+      </c>
+      <c r="C2825" t="inlineStr"/>
+      <c r="D2825" t="inlineStr"/>
+      <c r="E2825" t="inlineStr"/>
+      <c r="F2825" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2826">
+      <c r="A2826" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2826" t="inlineStr">
+        <is>
+          <t>[0, 17, 26]</t>
+        </is>
+      </c>
+      <c r="C2826" t="inlineStr"/>
+      <c r="D2826" t="inlineStr"/>
+      <c r="E2826" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2826" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2827">
+      <c r="A2827" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2827" t="inlineStr">
+        <is>
+          <t>[10, 21, 25]</t>
+        </is>
+      </c>
+      <c r="C2827" t="inlineStr"/>
+      <c r="D2827" t="inlineStr"/>
+      <c r="E2827" t="inlineStr"/>
+      <c r="F2827" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2828">
+      <c r="A2828" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2828" t="inlineStr">
+        <is>
+          <t>[20, 21, 31]</t>
+        </is>
+      </c>
+      <c r="C2828" t="inlineStr"/>
+      <c r="D2828" t="inlineStr"/>
+      <c r="E2828" t="inlineStr"/>
+      <c r="F2828" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2829">
+      <c r="A2829" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2829" t="inlineStr">
+        <is>
+          <t>[29, 30, 31]</t>
+        </is>
+      </c>
+      <c r="C2829" t="inlineStr"/>
+      <c r="D2829" t="inlineStr"/>
+      <c r="E2829" t="inlineStr"/>
+      <c r="F2829" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2830">
+      <c r="A2830" t="n">
+        <v>21</v>
+      </c>
+      <c r="B2830" t="inlineStr">
+        <is>
+          <t>[4, 12, 21]</t>
+        </is>
+      </c>
+      <c r="C2830" t="inlineStr"/>
+      <c r="D2830" t="inlineStr"/>
+      <c r="E2830" t="inlineStr"/>
+      <c r="F2830" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2831">
+      <c r="A2831" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2831" t="inlineStr">
+        <is>
+          <t>[12, 21, 28]</t>
+        </is>
+      </c>
+      <c r="C2831" t="inlineStr"/>
+      <c r="D2831" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2831" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2831" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2832">
+      <c r="A2832" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2832" t="inlineStr">
+        <is>
+          <t>[2, 15, 27]</t>
+        </is>
+      </c>
+      <c r="C2832" t="inlineStr"/>
+      <c r="D2832" t="inlineStr"/>
+      <c r="E2832" t="inlineStr"/>
+      <c r="F2832" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2833">
+      <c r="A2833" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2833" t="inlineStr">
+        <is>
+          <t>[9, 34, 36]</t>
+        </is>
+      </c>
+      <c r="C2833" t="inlineStr"/>
+      <c r="D2833" t="inlineStr"/>
+      <c r="E2833" t="inlineStr"/>
+      <c r="F2833" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2834">
+      <c r="A2834" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2834" t="inlineStr">
+        <is>
+          <t>[8, 9, 10]</t>
+        </is>
+      </c>
+      <c r="C2834" t="inlineStr"/>
+      <c r="D2834" t="inlineStr"/>
+      <c r="E2834" t="inlineStr"/>
+      <c r="F2834" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2835">
+      <c r="A2835" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2835" t="inlineStr">
+        <is>
+          <t>[4, 8, 10]</t>
+        </is>
+      </c>
+      <c r="C2835" t="inlineStr"/>
+      <c r="D2835" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2835" t="inlineStr"/>
+      <c r="F2835" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2836">
+      <c r="A2836" t="n">
+        <v>21</v>
+      </c>
+      <c r="B2836" t="inlineStr">
+        <is>
+          <t>[8, 10, 15]</t>
+        </is>
+      </c>
+      <c r="C2836" t="inlineStr"/>
+      <c r="D2836" t="inlineStr"/>
+      <c r="E2836" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2836" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2837">
+      <c r="A2837" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2837" t="inlineStr">
+        <is>
+          <t>[10, 15, 34]</t>
+        </is>
+      </c>
+      <c r="C2837" t="inlineStr"/>
+      <c r="D2837" t="inlineStr"/>
+      <c r="E2837" t="inlineStr"/>
+      <c r="F2837" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2838">
+      <c r="A2838" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2838" t="inlineStr">
+        <is>
+          <t>[1, 24, 35]</t>
+        </is>
+      </c>
+      <c r="C2838" t="inlineStr"/>
+      <c r="D2838" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2838" t="inlineStr"/>
+      <c r="F2838" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2839">
+      <c r="A2839" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2839" t="inlineStr">
+        <is>
+          <t>[19, 27, 33]</t>
+        </is>
+      </c>
+      <c r="C2839" t="inlineStr"/>
+      <c r="D2839" t="inlineStr"/>
+      <c r="E2839" t="inlineStr"/>
+      <c r="F2839" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2840">
+      <c r="A2840" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2840" t="inlineStr">
+        <is>
+          <t>[9, 19, 30]</t>
+        </is>
+      </c>
+      <c r="C2840" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2840" t="inlineStr"/>
+      <c r="E2840" t="inlineStr"/>
+      <c r="F2840" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2841">
+      <c r="A2841" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2841" t="inlineStr">
+        <is>
+          <t>[3, 6, 23]</t>
+        </is>
+      </c>
+      <c r="C2841" t="inlineStr"/>
+      <c r="D2841" t="inlineStr"/>
+      <c r="E2841" t="inlineStr"/>
+      <c r="F2841" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2842">
+      <c r="A2842" t="n">
+        <v>18</v>
+      </c>
+      <c r="B2842" t="inlineStr">
+        <is>
+          <t>[6, 23, 35]</t>
+        </is>
+      </c>
+      <c r="C2842" t="inlineStr"/>
+      <c r="D2842" t="inlineStr"/>
+      <c r="E2842" t="inlineStr"/>
+      <c r="F2842" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2843">
+      <c r="A2843" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2843" t="inlineStr">
+        <is>
+          <t>[6, 24, 29]</t>
+        </is>
+      </c>
+      <c r="C2843" t="inlineStr"/>
+      <c r="D2843" t="inlineStr"/>
+      <c r="E2843" t="inlineStr"/>
+      <c r="F2843" t="n">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
se encontro un modelo
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2843"/>
+  <dimension ref="A1:F3044"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44051,6 +44051,3602 @@
         <v>87</v>
       </c>
     </row>
+    <row r="2844">
+      <c r="A2844" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2844" t="inlineStr">
+        <is>
+          <t>[3, 6, 11, 22]</t>
+        </is>
+      </c>
+      <c r="C2844" t="inlineStr"/>
+      <c r="D2844" t="inlineStr"/>
+      <c r="E2844" t="inlineStr"/>
+      <c r="F2844" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2845">
+      <c r="A2845" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2845" t="inlineStr">
+        <is>
+          <t>[2, 3, 6, 12]</t>
+        </is>
+      </c>
+      <c r="C2845" t="inlineStr"/>
+      <c r="D2845" t="inlineStr"/>
+      <c r="E2845" t="inlineStr"/>
+      <c r="F2845" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2846">
+      <c r="A2846" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2846" t="inlineStr">
+        <is>
+          <t>[10, 14, 15, 21]</t>
+        </is>
+      </c>
+      <c r="C2846" t="inlineStr"/>
+      <c r="D2846" t="inlineStr"/>
+      <c r="E2846" t="inlineStr"/>
+      <c r="F2846" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2847">
+      <c r="A2847" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2847" t="inlineStr">
+        <is>
+          <t>[5, 15, 21, 35]</t>
+        </is>
+      </c>
+      <c r="C2847" t="inlineStr"/>
+      <c r="D2847" t="inlineStr"/>
+      <c r="E2847" t="inlineStr"/>
+      <c r="F2847" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2848">
+      <c r="A2848" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2848" t="inlineStr">
+        <is>
+          <t>[2, 21, 31, 35]</t>
+        </is>
+      </c>
+      <c r="C2848" t="inlineStr"/>
+      <c r="D2848" t="inlineStr"/>
+      <c r="E2848" t="inlineStr"/>
+      <c r="F2848" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2849">
+      <c r="A2849" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2849" t="inlineStr">
+        <is>
+          <t>[29, 30, 31, 35]</t>
+        </is>
+      </c>
+      <c r="C2849" t="inlineStr"/>
+      <c r="D2849" t="inlineStr"/>
+      <c r="E2849" t="inlineStr"/>
+      <c r="F2849" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2850">
+      <c r="A2850" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2850" t="inlineStr">
+        <is>
+          <t>[24, 29, 32, 35]</t>
+        </is>
+      </c>
+      <c r="C2850" t="inlineStr"/>
+      <c r="D2850" t="inlineStr"/>
+      <c r="E2850" t="inlineStr"/>
+      <c r="F2850" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2851">
+      <c r="A2851" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2851" t="inlineStr">
+        <is>
+          <t>[12, 15, 19, 25]</t>
+        </is>
+      </c>
+      <c r="C2851" t="inlineStr"/>
+      <c r="D2851" t="inlineStr"/>
+      <c r="E2851" t="inlineStr"/>
+      <c r="F2851" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2852">
+      <c r="A2852" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2852" t="inlineStr">
+        <is>
+          <t>[9, 25, 27, 32]</t>
+        </is>
+      </c>
+      <c r="C2852" t="inlineStr"/>
+      <c r="D2852" t="inlineStr"/>
+      <c r="E2852" t="inlineStr"/>
+      <c r="F2852" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2853">
+      <c r="A2853" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2853" t="inlineStr">
+        <is>
+          <t>[0, 26, 30, 31]</t>
+        </is>
+      </c>
+      <c r="C2853" t="inlineStr"/>
+      <c r="D2853" t="inlineStr"/>
+      <c r="E2853" t="inlineStr"/>
+      <c r="F2853" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2854">
+      <c r="A2854" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2854" t="inlineStr">
+        <is>
+          <t>[3, 7, 11, 17]</t>
+        </is>
+      </c>
+      <c r="C2854" t="inlineStr"/>
+      <c r="D2854" t="inlineStr"/>
+      <c r="E2854" t="inlineStr"/>
+      <c r="F2854" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2855">
+      <c r="A2855" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2855" t="inlineStr">
+        <is>
+          <t>[2, 3, 11, 12]</t>
+        </is>
+      </c>
+      <c r="C2855" t="inlineStr"/>
+      <c r="D2855" t="inlineStr"/>
+      <c r="E2855" t="inlineStr"/>
+      <c r="F2855" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2856">
+      <c r="A2856" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2856" t="inlineStr">
+        <is>
+          <t>[2, 5, 6, 8]</t>
+        </is>
+      </c>
+      <c r="C2856" t="inlineStr"/>
+      <c r="D2856" t="inlineStr"/>
+      <c r="E2856" t="inlineStr"/>
+      <c r="F2856" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2857">
+      <c r="A2857" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2857" t="inlineStr">
+        <is>
+          <t>[1, 3, 14, 21]</t>
+        </is>
+      </c>
+      <c r="C2857" t="inlineStr"/>
+      <c r="D2857" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2857" t="inlineStr"/>
+      <c r="F2857" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2858">
+      <c r="A2858" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2858" t="inlineStr">
+        <is>
+          <t>[5, 10, 14, 21]</t>
+        </is>
+      </c>
+      <c r="C2858" t="inlineStr"/>
+      <c r="D2858" t="inlineStr"/>
+      <c r="E2858" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2858" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2859">
+      <c r="A2859" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2859" t="inlineStr">
+        <is>
+          <t>[5, 10, 20, 34]</t>
+        </is>
+      </c>
+      <c r="C2859" t="inlineStr"/>
+      <c r="D2859" t="inlineStr"/>
+      <c r="E2859" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2859" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2860">
+      <c r="A2860" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2860" t="inlineStr">
+        <is>
+          <t>[1, 19, 25, 33]</t>
+        </is>
+      </c>
+      <c r="C2860" t="inlineStr"/>
+      <c r="D2860" t="inlineStr"/>
+      <c r="E2860" t="inlineStr"/>
+      <c r="F2860" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2861">
+      <c r="A2861" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2861" t="inlineStr">
+        <is>
+          <t>[12, 23, 27, 35]</t>
+        </is>
+      </c>
+      <c r="C2861" t="inlineStr"/>
+      <c r="D2861" t="inlineStr"/>
+      <c r="E2861" t="inlineStr"/>
+      <c r="F2861" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2862">
+      <c r="A2862" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2862" t="inlineStr">
+        <is>
+          <t>[6, 19, 33, 35]</t>
+        </is>
+      </c>
+      <c r="C2862" t="inlineStr"/>
+      <c r="D2862" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2862" t="inlineStr"/>
+      <c r="F2862" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2863">
+      <c r="A2863" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2863" t="inlineStr">
+        <is>
+          <t>[6, 7, 32, 33]</t>
+        </is>
+      </c>
+      <c r="C2863" t="inlineStr"/>
+      <c r="D2863" t="inlineStr"/>
+      <c r="E2863" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2863" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2864">
+      <c r="A2864" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2864" t="inlineStr">
+        <is>
+          <t>[3, 11, 21, 25]</t>
+        </is>
+      </c>
+      <c r="C2864" t="inlineStr"/>
+      <c r="D2864" t="inlineStr"/>
+      <c r="E2864" t="inlineStr"/>
+      <c r="F2864" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2865">
+      <c r="A2865" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2865" t="inlineStr">
+        <is>
+          <t>[3, 21, 22, 35]</t>
+        </is>
+      </c>
+      <c r="C2865" t="inlineStr"/>
+      <c r="D2865" t="inlineStr"/>
+      <c r="E2865" t="inlineStr"/>
+      <c r="F2865" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2866">
+      <c r="A2866" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2866" t="inlineStr">
+        <is>
+          <t>[1, 3, 14, 27]</t>
+        </is>
+      </c>
+      <c r="C2866" t="inlineStr"/>
+      <c r="D2866" t="inlineStr"/>
+      <c r="E2866" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2866" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2867">
+      <c r="A2867" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2867" t="inlineStr">
+        <is>
+          <t>[14, 16, 22, 29]</t>
+        </is>
+      </c>
+      <c r="C2867" t="inlineStr"/>
+      <c r="D2867" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2867" t="inlineStr"/>
+      <c r="F2867" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2868">
+      <c r="A2868" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2868" t="inlineStr">
+        <is>
+          <t>[14, 24, 27, 29]</t>
+        </is>
+      </c>
+      <c r="C2868" t="inlineStr"/>
+      <c r="D2868" t="inlineStr"/>
+      <c r="E2868" t="inlineStr"/>
+      <c r="F2868" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2869">
+      <c r="A2869" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2869" t="inlineStr">
+        <is>
+          <t>[1, 5, 10, 20]</t>
+        </is>
+      </c>
+      <c r="C2869" t="inlineStr"/>
+      <c r="D2869" t="inlineStr"/>
+      <c r="E2869" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2869" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2870">
+      <c r="A2870" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2870" t="inlineStr">
+        <is>
+          <t>[1, 5, 20, 21]</t>
+        </is>
+      </c>
+      <c r="C2870" t="inlineStr"/>
+      <c r="D2870" t="inlineStr"/>
+      <c r="E2870" t="inlineStr"/>
+      <c r="F2870" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2871">
+      <c r="A2871" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2871" t="inlineStr">
+        <is>
+          <t>[1, 19, 21, 31]</t>
+        </is>
+      </c>
+      <c r="C2871" t="inlineStr"/>
+      <c r="D2871" t="inlineStr"/>
+      <c r="E2871" t="inlineStr"/>
+      <c r="F2871" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2872">
+      <c r="A2872" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2872" t="inlineStr">
+        <is>
+          <t>[3, 6, 12, 18]</t>
+        </is>
+      </c>
+      <c r="C2872" t="inlineStr"/>
+      <c r="D2872" t="inlineStr"/>
+      <c r="E2872" t="inlineStr"/>
+      <c r="F2872" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2873">
+      <c r="A2873" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2873" t="inlineStr">
+        <is>
+          <t>[6, 19, 24, 33]</t>
+        </is>
+      </c>
+      <c r="C2873" t="inlineStr"/>
+      <c r="D2873" t="inlineStr"/>
+      <c r="E2873" t="inlineStr"/>
+      <c r="F2873" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2874">
+      <c r="A2874" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2874" t="inlineStr">
+        <is>
+          <t>[24, 29, 32, 33]</t>
+        </is>
+      </c>
+      <c r="C2874" t="inlineStr"/>
+      <c r="D2874" t="inlineStr"/>
+      <c r="E2874" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2874" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2875">
+      <c r="A2875" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2875" t="inlineStr">
+        <is>
+          <t>[3, 7, 11, 17]</t>
+        </is>
+      </c>
+      <c r="C2875" t="inlineStr"/>
+      <c r="D2875" t="inlineStr"/>
+      <c r="E2875" t="inlineStr"/>
+      <c r="F2875" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2876">
+      <c r="A2876" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2876" t="inlineStr">
+        <is>
+          <t>[2, 5, 8, 14]</t>
+        </is>
+      </c>
+      <c r="C2876" t="inlineStr"/>
+      <c r="D2876" t="inlineStr"/>
+      <c r="E2876" t="inlineStr"/>
+      <c r="F2876" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2877">
+      <c r="A2877" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2877" t="inlineStr">
+        <is>
+          <t>[0, 10, 14, 15]</t>
+        </is>
+      </c>
+      <c r="C2877" t="inlineStr"/>
+      <c r="D2877" t="inlineStr"/>
+      <c r="E2877" t="inlineStr"/>
+      <c r="F2877" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2878">
+      <c r="A2878" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2878" t="inlineStr">
+        <is>
+          <t>[10, 14, 15, 21]</t>
+        </is>
+      </c>
+      <c r="C2878" t="inlineStr"/>
+      <c r="D2878" t="inlineStr"/>
+      <c r="E2878" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2878" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2879">
+      <c r="A2879" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2879" t="inlineStr">
+        <is>
+          <t>[5, 10, 34, 35]</t>
+        </is>
+      </c>
+      <c r="C2879" t="inlineStr"/>
+      <c r="D2879" t="inlineStr"/>
+      <c r="E2879" t="inlineStr"/>
+      <c r="F2879" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2880">
+      <c r="A2880" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2880" t="inlineStr">
+        <is>
+          <t>[5, 19, 28, 33]</t>
+        </is>
+      </c>
+      <c r="C2880" t="inlineStr"/>
+      <c r="D2880" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2880" t="inlineStr"/>
+      <c r="F2880" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2881">
+      <c r="A2881" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2881" t="inlineStr">
+        <is>
+          <t>[9, 23, 27, 35]</t>
+        </is>
+      </c>
+      <c r="C2881" t="inlineStr"/>
+      <c r="D2881" t="inlineStr"/>
+      <c r="E2881" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2881" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2882">
+      <c r="A2882" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2882" t="inlineStr">
+        <is>
+          <t>[6, 19, 23, 35]</t>
+        </is>
+      </c>
+      <c r="C2882" t="inlineStr"/>
+      <c r="D2882" t="inlineStr"/>
+      <c r="E2882" t="inlineStr"/>
+      <c r="F2882" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2883">
+      <c r="A2883" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2883" t="inlineStr">
+        <is>
+          <t>[6, 19, 24, 33]</t>
+        </is>
+      </c>
+      <c r="C2883" t="inlineStr"/>
+      <c r="D2883" t="inlineStr"/>
+      <c r="E2883" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2883" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2884">
+      <c r="A2884" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2884" t="inlineStr">
+        <is>
+          <t>[17, 21, 25, 33]</t>
+        </is>
+      </c>
+      <c r="C2884" t="inlineStr"/>
+      <c r="D2884" t="inlineStr"/>
+      <c r="E2884" t="inlineStr"/>
+      <c r="F2884" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2885">
+      <c r="A2885" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2885" t="inlineStr">
+        <is>
+          <t>[3, 9, 33, 35]</t>
+        </is>
+      </c>
+      <c r="C2885" t="inlineStr"/>
+      <c r="D2885" t="inlineStr"/>
+      <c r="E2885" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2885" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2886">
+      <c r="A2886" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2886" t="inlineStr">
+        <is>
+          <t>[14, 22, 27, 29]</t>
+        </is>
+      </c>
+      <c r="C2886" t="inlineStr"/>
+      <c r="D2886" t="inlineStr"/>
+      <c r="E2886" t="inlineStr"/>
+      <c r="F2886" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2887">
+      <c r="A2887" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2887" t="inlineStr">
+        <is>
+          <t>[3, 6, 8, 22]</t>
+        </is>
+      </c>
+      <c r="C2887" t="inlineStr"/>
+      <c r="D2887" t="inlineStr"/>
+      <c r="E2887" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2887" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2888">
+      <c r="A2888" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2888" t="inlineStr">
+        <is>
+          <t>[7, 8, 11, 24]</t>
+        </is>
+      </c>
+      <c r="C2888" t="inlineStr"/>
+      <c r="D2888" t="inlineStr"/>
+      <c r="E2888" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2888" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2889">
+      <c r="A2889" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2889" t="inlineStr">
+        <is>
+          <t>[7, 8, 11, 24]</t>
+        </is>
+      </c>
+      <c r="C2889" t="inlineStr"/>
+      <c r="D2889" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2889" t="inlineStr"/>
+      <c r="F2889" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2890">
+      <c r="A2890" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2890" t="inlineStr">
+        <is>
+          <t>[8, 10, 11, 14]</t>
+        </is>
+      </c>
+      <c r="C2890" t="inlineStr"/>
+      <c r="D2890" t="inlineStr"/>
+      <c r="E2890" t="inlineStr"/>
+      <c r="F2890" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2891">
+      <c r="A2891" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2891" t="inlineStr">
+        <is>
+          <t>[0, 10, 14, 17]</t>
+        </is>
+      </c>
+      <c r="C2891" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2891" t="inlineStr"/>
+      <c r="E2891" t="inlineStr"/>
+      <c r="F2891" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2892">
+      <c r="A2892" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2892" t="inlineStr">
+        <is>
+          <t>[10, 14, 15, 18]</t>
+        </is>
+      </c>
+      <c r="C2892" t="inlineStr"/>
+      <c r="D2892" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2892" t="inlineStr"/>
+      <c r="F2892" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2893">
+      <c r="A2893" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2893" t="inlineStr">
+        <is>
+          <t>[14, 18, 19, 33]</t>
+        </is>
+      </c>
+      <c r="C2893" t="inlineStr"/>
+      <c r="D2893" t="inlineStr"/>
+      <c r="E2893" t="inlineStr"/>
+      <c r="F2893" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2894">
+      <c r="A2894" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2894" t="inlineStr">
+        <is>
+          <t>[14, 19, 24, 29]</t>
+        </is>
+      </c>
+      <c r="C2894" t="inlineStr"/>
+      <c r="D2894" t="inlineStr"/>
+      <c r="E2894" t="inlineStr"/>
+      <c r="F2894" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2895">
+      <c r="A2895" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2895" t="inlineStr">
+        <is>
+          <t>[7, 16, 24, 29]</t>
+        </is>
+      </c>
+      <c r="C2895" t="inlineStr"/>
+      <c r="D2895" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2895" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2895" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2896">
+      <c r="A2896" t="n">
+        <v>18</v>
+      </c>
+      <c r="B2896" t="inlineStr">
+        <is>
+          <t>[7, 16, 24, 29]</t>
+        </is>
+      </c>
+      <c r="C2896" t="inlineStr"/>
+      <c r="D2896" t="inlineStr"/>
+      <c r="E2896" t="inlineStr"/>
+      <c r="F2896" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2897">
+      <c r="A2897" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2897" t="inlineStr">
+        <is>
+          <t>[14, 16, 22, 29]</t>
+        </is>
+      </c>
+      <c r="C2897" t="inlineStr"/>
+      <c r="D2897" t="inlineStr"/>
+      <c r="E2897" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2897" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2898">
+      <c r="A2898" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2898" t="inlineStr">
+        <is>
+          <t>[5, 10, 14, 29]</t>
+        </is>
+      </c>
+      <c r="C2898" t="inlineStr"/>
+      <c r="D2898" t="inlineStr"/>
+      <c r="E2898" t="inlineStr"/>
+      <c r="F2898" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2899">
+      <c r="A2899" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2899" t="inlineStr">
+        <is>
+          <t>[1, 5, 20, 25]</t>
+        </is>
+      </c>
+      <c r="C2899" t="inlineStr"/>
+      <c r="D2899" t="inlineStr"/>
+      <c r="E2899" t="inlineStr"/>
+      <c r="F2899" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2900">
+      <c r="A2900" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2900" t="inlineStr">
+        <is>
+          <t>[1, 20, 25, 27]</t>
+        </is>
+      </c>
+      <c r="C2900" t="inlineStr"/>
+      <c r="D2900" t="inlineStr"/>
+      <c r="E2900" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2900" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2901">
+      <c r="A2901" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2901" t="inlineStr">
+        <is>
+          <t>[3, 12, 19, 27]</t>
+        </is>
+      </c>
+      <c r="C2901" t="inlineStr"/>
+      <c r="D2901" t="inlineStr"/>
+      <c r="E2901" t="inlineStr"/>
+      <c r="F2901" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2902">
+      <c r="A2902" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2902" t="inlineStr">
+        <is>
+          <t>[6, 19, 35, 36]</t>
+        </is>
+      </c>
+      <c r="C2902" t="inlineStr"/>
+      <c r="D2902" t="inlineStr"/>
+      <c r="E2902" t="inlineStr"/>
+      <c r="F2902" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2903">
+      <c r="A2903" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2903" t="inlineStr">
+        <is>
+          <t>[6, 7, 32, 33]</t>
+        </is>
+      </c>
+      <c r="C2903" t="inlineStr"/>
+      <c r="D2903" t="inlineStr"/>
+      <c r="E2903" t="inlineStr"/>
+      <c r="F2903" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2904">
+      <c r="A2904" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2904" t="inlineStr">
+        <is>
+          <t>[3, 7, 11, 12]</t>
+        </is>
+      </c>
+      <c r="C2904" t="inlineStr"/>
+      <c r="D2904" t="inlineStr"/>
+      <c r="E2904" t="inlineStr"/>
+      <c r="F2904" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2905">
+      <c r="A2905" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2905" t="inlineStr">
+        <is>
+          <t>[2, 3, 6, 12]</t>
+        </is>
+      </c>
+      <c r="C2905" t="inlineStr"/>
+      <c r="D2905" t="inlineStr"/>
+      <c r="E2905" t="inlineStr"/>
+      <c r="F2905" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2906">
+      <c r="A2906" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2906" t="inlineStr">
+        <is>
+          <t>[3, 10, 21, 26]</t>
+        </is>
+      </c>
+      <c r="C2906" t="inlineStr"/>
+      <c r="D2906" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2906" t="inlineStr"/>
+      <c r="F2906" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2907">
+      <c r="A2907" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2907" t="inlineStr">
+        <is>
+          <t>[1, 25, 28, 33]</t>
+        </is>
+      </c>
+      <c r="C2907" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2907" t="inlineStr"/>
+      <c r="E2907" t="inlineStr"/>
+      <c r="F2907" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2908">
+      <c r="A2908" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2908" t="inlineStr">
+        <is>
+          <t>[1, 19, 27, 28]</t>
+        </is>
+      </c>
+      <c r="C2908" t="inlineStr"/>
+      <c r="D2908" t="inlineStr"/>
+      <c r="E2908" t="inlineStr"/>
+      <c r="F2908" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2909">
+      <c r="A2909" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2909" t="inlineStr">
+        <is>
+          <t>[6, 19, 23, 35]</t>
+        </is>
+      </c>
+      <c r="C2909" t="inlineStr"/>
+      <c r="D2909" t="inlineStr"/>
+      <c r="E2909" t="inlineStr"/>
+      <c r="F2909" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2910">
+      <c r="A2910" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2910" t="inlineStr">
+        <is>
+          <t>[6, 19, 24, 33]</t>
+        </is>
+      </c>
+      <c r="C2910" t="inlineStr"/>
+      <c r="D2910" t="inlineStr"/>
+      <c r="E2910" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2910" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2911">
+      <c r="A2911" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2911" t="inlineStr">
+        <is>
+          <t>[6, 7, 30, 33]</t>
+        </is>
+      </c>
+      <c r="C2911" t="inlineStr"/>
+      <c r="D2911" t="inlineStr"/>
+      <c r="E2911" t="inlineStr"/>
+      <c r="F2911" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2912">
+      <c r="A2912" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2912" t="inlineStr">
+        <is>
+          <t>[3, 11, 12, 21]</t>
+        </is>
+      </c>
+      <c r="C2912" t="inlineStr"/>
+      <c r="D2912" t="inlineStr"/>
+      <c r="E2912" t="inlineStr"/>
+      <c r="F2912" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2913">
+      <c r="A2913" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2913" t="inlineStr">
+        <is>
+          <t>[1, 3, 14, 27]</t>
+        </is>
+      </c>
+      <c r="C2913" t="inlineStr"/>
+      <c r="D2913" t="inlineStr"/>
+      <c r="E2913" t="inlineStr"/>
+      <c r="F2913" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2914">
+      <c r="A2914" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2914" t="inlineStr">
+        <is>
+          <t>[3, 14, 22, 29]</t>
+        </is>
+      </c>
+      <c r="C2914" t="inlineStr"/>
+      <c r="D2914" t="inlineStr"/>
+      <c r="E2914" t="inlineStr"/>
+      <c r="F2914" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2915">
+      <c r="A2915" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2915" t="inlineStr">
+        <is>
+          <t>[7, 8, 24, 29]</t>
+        </is>
+      </c>
+      <c r="C2915" t="inlineStr"/>
+      <c r="D2915" t="inlineStr"/>
+      <c r="E2915" t="inlineStr"/>
+      <c r="F2915" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2916">
+      <c r="A2916" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2916" t="inlineStr">
+        <is>
+          <t>[0, 6, 8, 11, 14, 18]</t>
+        </is>
+      </c>
+      <c r="C2916" t="inlineStr"/>
+      <c r="D2916" t="inlineStr"/>
+      <c r="E2916" t="inlineStr"/>
+      <c r="F2916" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2917">
+      <c r="A2917" t="n">
+        <v>21</v>
+      </c>
+      <c r="B2917" t="inlineStr">
+        <is>
+          <t>[6, 12, 14, 16, 18, 29]</t>
+        </is>
+      </c>
+      <c r="C2917" t="inlineStr"/>
+      <c r="D2917" t="inlineStr"/>
+      <c r="E2917" t="inlineStr"/>
+      <c r="F2917" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2918">
+      <c r="A2918" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2918" t="inlineStr">
+        <is>
+          <t>[12, 13, 14, 18, 21, 29]</t>
+        </is>
+      </c>
+      <c r="C2918" t="inlineStr"/>
+      <c r="D2918" t="inlineStr"/>
+      <c r="E2918" t="inlineStr"/>
+      <c r="F2918" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2919">
+      <c r="A2919" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2919" t="inlineStr">
+        <is>
+          <t>[5, 13, 14, 18, 21, 29]</t>
+        </is>
+      </c>
+      <c r="C2919" t="inlineStr"/>
+      <c r="D2919" t="inlineStr"/>
+      <c r="E2919" t="inlineStr"/>
+      <c r="F2919" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2920">
+      <c r="A2920" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2920" t="inlineStr">
+        <is>
+          <t>[1, 5, 20, 27, 33, 35]</t>
+        </is>
+      </c>
+      <c r="C2920" t="inlineStr"/>
+      <c r="D2920" t="inlineStr"/>
+      <c r="E2920" t="inlineStr"/>
+      <c r="F2920" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2921">
+      <c r="A2921" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2921" t="inlineStr">
+        <is>
+          <t>[1, 3, 5, 22, 23, 27]</t>
+        </is>
+      </c>
+      <c r="C2921" t="inlineStr"/>
+      <c r="D2921" t="inlineStr"/>
+      <c r="E2921" t="inlineStr"/>
+      <c r="F2921" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2922">
+      <c r="A2922" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2922" t="inlineStr">
+        <is>
+          <t>[16, 22, 23, 24, 29, 30]</t>
+        </is>
+      </c>
+      <c r="C2922" t="inlineStr"/>
+      <c r="D2922" t="inlineStr"/>
+      <c r="E2922" t="inlineStr"/>
+      <c r="F2922" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2923">
+      <c r="A2923" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2923" t="inlineStr">
+        <is>
+          <t>[6, 7, 8, 22, 24, 30]</t>
+        </is>
+      </c>
+      <c r="C2923" t="inlineStr"/>
+      <c r="D2923" t="inlineStr"/>
+      <c r="E2923" t="inlineStr"/>
+      <c r="F2923" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2924">
+      <c r="A2924" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2924" t="inlineStr">
+        <is>
+          <t>[6, 7, 8, 11, 22, 24]</t>
+        </is>
+      </c>
+      <c r="C2924" t="inlineStr"/>
+      <c r="D2924" t="inlineStr"/>
+      <c r="E2924" t="inlineStr"/>
+      <c r="F2924" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2925">
+      <c r="A2925" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2925" t="inlineStr">
+        <is>
+          <t>[0, 6, 8, 10, 18, 22]</t>
+        </is>
+      </c>
+      <c r="C2925" t="inlineStr"/>
+      <c r="D2925" t="inlineStr"/>
+      <c r="E2925" t="inlineStr"/>
+      <c r="F2925" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2926">
+      <c r="A2926" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2926" t="inlineStr">
+        <is>
+          <t>[0, 8, 10, 15, 18, 27]</t>
+        </is>
+      </c>
+      <c r="C2926" t="inlineStr"/>
+      <c r="D2926" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2926" t="inlineStr"/>
+      <c r="F2926" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2927">
+      <c r="A2927" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2927" t="inlineStr">
+        <is>
+          <t>[8, 10, 14, 18, 19, 34]</t>
+        </is>
+      </c>
+      <c r="C2927" t="inlineStr"/>
+      <c r="D2927" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2927" t="inlineStr"/>
+      <c r="F2927" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2928">
+      <c r="A2928" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2928" t="inlineStr">
+        <is>
+          <t>[14, 16, 18, 19, 34, 35]</t>
+        </is>
+      </c>
+      <c r="C2928" t="inlineStr"/>
+      <c r="D2928" t="inlineStr"/>
+      <c r="E2928" t="inlineStr"/>
+      <c r="F2928" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2929">
+      <c r="A2929" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2929" t="inlineStr">
+        <is>
+          <t>[8, 12, 13, 14, 18, 21]</t>
+        </is>
+      </c>
+      <c r="C2929" t="inlineStr"/>
+      <c r="D2929" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2929" t="inlineStr"/>
+      <c r="F2929" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2930">
+      <c r="A2930" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2930" t="inlineStr">
+        <is>
+          <t>[5, 14, 18, 21, 26, 29]</t>
+        </is>
+      </c>
+      <c r="C2930" t="inlineStr"/>
+      <c r="D2930" t="inlineStr"/>
+      <c r="E2930" t="inlineStr"/>
+      <c r="F2930" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2931">
+      <c r="A2931" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2931" t="inlineStr">
+        <is>
+          <t>[1, 5, 14, 27, 34, 35]</t>
+        </is>
+      </c>
+      <c r="C2931" t="inlineStr"/>
+      <c r="D2931" t="inlineStr"/>
+      <c r="E2931" t="inlineStr"/>
+      <c r="F2931" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2932">
+      <c r="A2932" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2932" t="inlineStr">
+        <is>
+          <t>[3, 5, 14, 23, 27, 29]</t>
+        </is>
+      </c>
+      <c r="C2932" t="inlineStr"/>
+      <c r="D2932" t="inlineStr"/>
+      <c r="E2932" t="inlineStr"/>
+      <c r="F2932" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2933">
+      <c r="A2933" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2933" t="inlineStr">
+        <is>
+          <t>[3, 6, 16, 24, 29, 30]</t>
+        </is>
+      </c>
+      <c r="C2933" t="inlineStr"/>
+      <c r="D2933" t="inlineStr"/>
+      <c r="E2933" t="inlineStr"/>
+      <c r="F2933" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2934">
+      <c r="A2934" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2934" t="inlineStr">
+        <is>
+          <t>[6, 7, 11, 12, 22, 25]</t>
+        </is>
+      </c>
+      <c r="C2934" t="inlineStr"/>
+      <c r="D2934" t="inlineStr"/>
+      <c r="E2934" t="inlineStr"/>
+      <c r="F2934" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2935">
+      <c r="A2935" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2935" t="inlineStr">
+        <is>
+          <t>[11, 12, 13, 23, 25, 26]</t>
+        </is>
+      </c>
+      <c r="C2935" t="inlineStr"/>
+      <c r="D2935" t="inlineStr"/>
+      <c r="E2935" t="inlineStr"/>
+      <c r="F2935" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2936">
+      <c r="A2936" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2936" t="inlineStr">
+        <is>
+          <t>[0, 5, 20, 25, 32, 33]</t>
+        </is>
+      </c>
+      <c r="C2936" t="inlineStr"/>
+      <c r="D2936" t="inlineStr"/>
+      <c r="E2936" t="inlineStr"/>
+      <c r="F2936" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2937">
+      <c r="A2937" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2937" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 25, 31, 33]</t>
+        </is>
+      </c>
+      <c r="C2937" t="inlineStr"/>
+      <c r="D2937" t="inlineStr"/>
+      <c r="E2937" t="inlineStr"/>
+      <c r="F2937" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2938">
+      <c r="A2938" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2938" t="inlineStr">
+        <is>
+          <t>[6, 12, 15, 18, 19, 30]</t>
+        </is>
+      </c>
+      <c r="C2938" t="inlineStr"/>
+      <c r="D2938" t="inlineStr"/>
+      <c r="E2938" t="inlineStr"/>
+      <c r="F2938" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2939">
+      <c r="A2939" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2939" t="inlineStr">
+        <is>
+          <t>[3, 6, 7, 12, 13, 19]</t>
+        </is>
+      </c>
+      <c r="C2939" t="inlineStr"/>
+      <c r="D2939" t="inlineStr"/>
+      <c r="E2939" t="inlineStr"/>
+      <c r="F2939" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2940">
+      <c r="A2940" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2940" t="inlineStr">
+        <is>
+          <t>[6, 7, 10, 13, 24, 33]</t>
+        </is>
+      </c>
+      <c r="C2940" t="inlineStr"/>
+      <c r="D2940" t="inlineStr"/>
+      <c r="E2940" t="inlineStr"/>
+      <c r="F2940" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2941" t="inlineStr">
+        <is>
+          <t>[10, 17, 20, 21, 25, 33]</t>
+        </is>
+      </c>
+      <c r="C2941" t="inlineStr"/>
+      <c r="D2941" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2941" t="inlineStr"/>
+      <c r="F2941" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2942" t="inlineStr">
+        <is>
+          <t>[3, 9, 10, 11, 16, 25]</t>
+        </is>
+      </c>
+      <c r="C2942" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2942" t="inlineStr"/>
+      <c r="E2942" t="inlineStr"/>
+      <c r="F2942" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2943" t="inlineStr">
+        <is>
+          <t>[4, 5, 8, 20, 21, 32]</t>
+        </is>
+      </c>
+      <c r="C2943" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2943" t="inlineStr"/>
+      <c r="E2943" t="inlineStr"/>
+      <c r="F2943" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2944" t="inlineStr">
+        <is>
+          <t>[2, 8, 17, 20, 21, 30]</t>
+        </is>
+      </c>
+      <c r="C2944" t="inlineStr"/>
+      <c r="D2944" t="inlineStr"/>
+      <c r="E2944" t="inlineStr"/>
+      <c r="F2944" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2945" t="inlineStr">
+        <is>
+          <t>[2, 15, 18, 21, 30, 31]</t>
+        </is>
+      </c>
+      <c r="C2945" t="inlineStr"/>
+      <c r="D2945" t="inlineStr"/>
+      <c r="E2945" t="inlineStr"/>
+      <c r="F2945" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2946" t="inlineStr">
+        <is>
+          <t>[12, 15, 18, 27, 29, 35]</t>
+        </is>
+      </c>
+      <c r="C2946" t="inlineStr"/>
+      <c r="D2946" t="inlineStr"/>
+      <c r="E2946" t="inlineStr"/>
+      <c r="F2946" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2947" t="inlineStr">
+        <is>
+          <t>[11, 12, 15, 27, 28, 35]</t>
+        </is>
+      </c>
+      <c r="C2947" t="inlineStr"/>
+      <c r="D2947" t="inlineStr"/>
+      <c r="E2947" t="inlineStr"/>
+      <c r="F2947" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2948" t="inlineStr">
+        <is>
+          <t>[7, 14, 27, 30, 32, 34]</t>
+        </is>
+      </c>
+      <c r="C2948" t="inlineStr"/>
+      <c r="D2948" t="inlineStr"/>
+      <c r="E2948" t="inlineStr"/>
+      <c r="F2948" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2949" t="inlineStr">
+        <is>
+          <t>[7, 10, 27, 30, 34, 36]</t>
+        </is>
+      </c>
+      <c r="C2949" t="inlineStr"/>
+      <c r="D2949" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2949" t="inlineStr"/>
+      <c r="F2949" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2950" t="inlineStr">
+        <is>
+          <t>[10, 14, 17, 21, 22, 26]</t>
+        </is>
+      </c>
+      <c r="C2950" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2950" t="inlineStr"/>
+      <c r="E2950" t="inlineStr"/>
+      <c r="F2950" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2951" t="inlineStr">
+        <is>
+          <t>[2, 10, 12, 13, 18, 21]</t>
+        </is>
+      </c>
+      <c r="C2951" t="inlineStr"/>
+      <c r="D2951" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2951" t="inlineStr"/>
+      <c r="F2951" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2952" t="inlineStr">
+        <is>
+          <t>[1, 3, 14, 22, 27, 35]</t>
+        </is>
+      </c>
+      <c r="C2952" t="inlineStr"/>
+      <c r="D2952" t="inlineStr"/>
+      <c r="E2952" t="inlineStr"/>
+      <c r="F2952" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2953">
+      <c r="A2953" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2953" t="inlineStr">
+        <is>
+          <t>[3, 7, 14, 16, 19, 29]</t>
+        </is>
+      </c>
+      <c r="C2953" t="inlineStr"/>
+      <c r="D2953" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2953" t="inlineStr"/>
+      <c r="F2953" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2954" t="inlineStr">
+        <is>
+          <t>[0, 7, 12, 14, 16, 29]</t>
+        </is>
+      </c>
+      <c r="C2954" t="inlineStr"/>
+      <c r="D2954" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2954" t="inlineStr"/>
+      <c r="F2954" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2955" t="inlineStr">
+        <is>
+          <t>[1, 12, 14, 16, 19, 29]</t>
+        </is>
+      </c>
+      <c r="C2955" t="inlineStr"/>
+      <c r="D2955" t="inlineStr"/>
+      <c r="E2955" t="inlineStr"/>
+      <c r="F2955" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2956" t="inlineStr">
+        <is>
+          <t>[3, 14, 16, 19, 27, 29]</t>
+        </is>
+      </c>
+      <c r="C2956" t="inlineStr"/>
+      <c r="D2956" t="inlineStr"/>
+      <c r="E2956" t="inlineStr"/>
+      <c r="F2956" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2957" t="inlineStr">
+        <is>
+          <t>[3, 6, 14, 22, 29, 30]</t>
+        </is>
+      </c>
+      <c r="C2957" t="inlineStr"/>
+      <c r="D2957" t="inlineStr"/>
+      <c r="E2957" t="inlineStr"/>
+      <c r="F2957" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2958" t="inlineStr">
+        <is>
+          <t>[6, 7, 8, 11, 12, 22]</t>
+        </is>
+      </c>
+      <c r="C2958" t="inlineStr"/>
+      <c r="D2958" t="inlineStr"/>
+      <c r="E2958" t="inlineStr"/>
+      <c r="F2958" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2959" t="inlineStr">
+        <is>
+          <t>[2, 6, 11, 12, 14, 23]</t>
+        </is>
+      </c>
+      <c r="C2959" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2959" t="inlineStr"/>
+      <c r="E2959" t="inlineStr"/>
+      <c r="F2959" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2960" t="inlineStr">
+        <is>
+          <t>[3, 5, 10, 14, 24, 26]</t>
+        </is>
+      </c>
+      <c r="C2960" t="inlineStr"/>
+      <c r="D2960" t="inlineStr"/>
+      <c r="E2960" t="inlineStr"/>
+      <c r="F2960" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2961" t="inlineStr">
+        <is>
+          <t>[0, 4, 5, 32]</t>
+        </is>
+      </c>
+      <c r="C2961" t="inlineStr"/>
+      <c r="D2961" t="inlineStr"/>
+      <c r="E2961" t="inlineStr"/>
+      <c r="F2961" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2962" t="inlineStr">
+        <is>
+          <t>[3, 5, 8, 9]</t>
+        </is>
+      </c>
+      <c r="C2962" t="inlineStr"/>
+      <c r="D2962" t="inlineStr"/>
+      <c r="E2962" t="inlineStr"/>
+      <c r="F2962" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2963">
+      <c r="A2963" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2963" t="inlineStr">
+        <is>
+          <t>[13, 27, 30, 34]</t>
+        </is>
+      </c>
+      <c r="C2963" t="inlineStr"/>
+      <c r="D2963" t="inlineStr"/>
+      <c r="E2963" t="inlineStr"/>
+      <c r="F2963" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2964">
+      <c r="A2964" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2964" t="inlineStr">
+        <is>
+          <t>[10, 19, 33, 34]</t>
+        </is>
+      </c>
+      <c r="C2964" t="inlineStr"/>
+      <c r="D2964" t="inlineStr"/>
+      <c r="E2964" t="inlineStr"/>
+      <c r="F2964" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2965">
+      <c r="A2965" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2965" t="inlineStr">
+        <is>
+          <t>[6, 10, 28, 33]</t>
+        </is>
+      </c>
+      <c r="C2965" t="inlineStr"/>
+      <c r="D2965" t="inlineStr"/>
+      <c r="E2965" t="inlineStr"/>
+      <c r="F2965" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2966">
+      <c r="A2966" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2966" t="inlineStr">
+        <is>
+          <t>[3, 9, 23, 33]</t>
+        </is>
+      </c>
+      <c r="C2966" t="inlineStr"/>
+      <c r="D2966" t="inlineStr"/>
+      <c r="E2966" t="inlineStr"/>
+      <c r="F2966" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2967">
+      <c r="A2967" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2967" t="inlineStr">
+        <is>
+          <t>[1, 22, 27, 35]</t>
+        </is>
+      </c>
+      <c r="C2967" t="inlineStr"/>
+      <c r="D2967" t="inlineStr"/>
+      <c r="E2967" t="inlineStr"/>
+      <c r="F2967" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2968">
+      <c r="A2968" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2968" t="inlineStr">
+        <is>
+          <t>[0, 1, 14, 22]</t>
+        </is>
+      </c>
+      <c r="C2968" t="inlineStr"/>
+      <c r="D2968" t="inlineStr"/>
+      <c r="E2968" t="inlineStr"/>
+      <c r="F2968" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2969">
+      <c r="A2969" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2969" t="inlineStr">
+        <is>
+          <t>[6, 7, 23, 35]</t>
+        </is>
+      </c>
+      <c r="C2969" t="inlineStr"/>
+      <c r="D2969" t="inlineStr"/>
+      <c r="E2969" t="inlineStr"/>
+      <c r="F2969" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2970">
+      <c r="A2970" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2970" t="inlineStr">
+        <is>
+          <t>[12, 23, 25, 29]</t>
+        </is>
+      </c>
+      <c r="C2970" t="inlineStr"/>
+      <c r="D2970" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2970" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2970" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2971">
+      <c r="A2971" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2971" t="inlineStr">
+        <is>
+          <t>[1, 10, 20, 33]</t>
+        </is>
+      </c>
+      <c r="C2971" t="inlineStr"/>
+      <c r="D2971" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2971" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2971" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2972">
+      <c r="A2972" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2972" t="inlineStr">
+        <is>
+          <t>[0, 14, 20, 28]</t>
+        </is>
+      </c>
+      <c r="C2972" t="inlineStr"/>
+      <c r="D2972" t="inlineStr"/>
+      <c r="E2972" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2972" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2973">
+      <c r="A2973" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2973" t="inlineStr">
+        <is>
+          <t>[0, 3, 5, 32]</t>
+        </is>
+      </c>
+      <c r="C2973" t="inlineStr"/>
+      <c r="D2973" t="inlineStr"/>
+      <c r="E2973" t="inlineStr"/>
+      <c r="F2973" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2974">
+      <c r="A2974" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2974" t="inlineStr">
+        <is>
+          <t>[3, 21, 30, 34]</t>
+        </is>
+      </c>
+      <c r="C2974" t="inlineStr"/>
+      <c r="D2974" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2974" t="inlineStr"/>
+      <c r="F2974" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2975">
+      <c r="A2975" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2975" t="inlineStr">
+        <is>
+          <t>[12, 27, 30, 34]</t>
+        </is>
+      </c>
+      <c r="C2975" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D2975" t="inlineStr"/>
+      <c r="E2975" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2975" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2976">
+      <c r="A2976" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2976" t="inlineStr">
+        <is>
+          <t>[7, 23, 24, 30]</t>
+        </is>
+      </c>
+      <c r="C2976" t="inlineStr"/>
+      <c r="D2976" t="inlineStr"/>
+      <c r="E2976" t="inlineStr"/>
+      <c r="F2976" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2977">
+      <c r="A2977" t="n">
+        <v>35</v>
+      </c>
+      <c r="B2977" t="inlineStr">
+        <is>
+          <t>[3, 7, 24, 30]</t>
+        </is>
+      </c>
+      <c r="C2977" t="inlineStr"/>
+      <c r="D2977" t="inlineStr"/>
+      <c r="E2977" t="inlineStr"/>
+      <c r="F2977" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2978">
+      <c r="A2978" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2978" t="inlineStr">
+        <is>
+          <t>[7, 23, 32, 34]</t>
+        </is>
+      </c>
+      <c r="C2978" t="inlineStr"/>
+      <c r="D2978" t="inlineStr"/>
+      <c r="E2978" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2978" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2979">
+      <c r="A2979" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2979" t="inlineStr">
+        <is>
+          <t>[4, 6, 8, 24]</t>
+        </is>
+      </c>
+      <c r="C2979" t="inlineStr"/>
+      <c r="D2979" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2979" t="inlineStr"/>
+      <c r="F2979" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2980">
+      <c r="A2980" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2980" t="inlineStr">
+        <is>
+          <t>[4, 10, 17, 22]</t>
+        </is>
+      </c>
+      <c r="C2980" t="inlineStr"/>
+      <c r="D2980" t="inlineStr"/>
+      <c r="E2980" t="inlineStr"/>
+      <c r="F2980" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2981">
+      <c r="A2981" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2981" t="inlineStr">
+        <is>
+          <t>[6, 10, 15, 17]</t>
+        </is>
+      </c>
+      <c r="C2981" t="inlineStr"/>
+      <c r="D2981" t="inlineStr"/>
+      <c r="E2981" t="inlineStr"/>
+      <c r="F2981" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2982">
+      <c r="A2982" t="n">
+        <v>18</v>
+      </c>
+      <c r="B2982" t="inlineStr">
+        <is>
+          <t>[5, 8, 10, 14]</t>
+        </is>
+      </c>
+      <c r="C2982" t="inlineStr"/>
+      <c r="D2982" t="inlineStr"/>
+      <c r="E2982" t="inlineStr"/>
+      <c r="F2982" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2983">
+      <c r="A2983" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2983" t="inlineStr">
+        <is>
+          <t>[5, 8, 10, 14]</t>
+        </is>
+      </c>
+      <c r="C2983" t="inlineStr"/>
+      <c r="D2983" t="inlineStr"/>
+      <c r="E2983" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2983" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2984">
+      <c r="A2984" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2984" t="inlineStr">
+        <is>
+          <t>[14, 15, 17, 18]</t>
+        </is>
+      </c>
+      <c r="C2984" t="inlineStr"/>
+      <c r="D2984" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2984" t="inlineStr"/>
+      <c r="F2984" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2985">
+      <c r="A2985" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2985" t="inlineStr">
+        <is>
+          <t>[14, 18, 33, 35]</t>
+        </is>
+      </c>
+      <c r="C2985" t="inlineStr"/>
+      <c r="D2985" t="inlineStr"/>
+      <c r="E2985" t="inlineStr"/>
+      <c r="F2985" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2986">
+      <c r="A2986" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2986" t="inlineStr">
+        <is>
+          <t>[5, 21, 31, 34]</t>
+        </is>
+      </c>
+      <c r="C2986" t="inlineStr"/>
+      <c r="D2986" t="inlineStr"/>
+      <c r="E2986" t="inlineStr"/>
+      <c r="F2986" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2987">
+      <c r="A2987" t="n">
+        <v>32</v>
+      </c>
+      <c r="B2987" t="inlineStr">
+        <is>
+          <t>[19, 20, 28, 33]</t>
+        </is>
+      </c>
+      <c r="C2987" t="inlineStr"/>
+      <c r="D2987" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2987" t="inlineStr"/>
+      <c r="F2987" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2988">
+      <c r="A2988" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2988" t="inlineStr">
+        <is>
+          <t>[0, 3, 13, 19]</t>
+        </is>
+      </c>
+      <c r="C2988" t="inlineStr"/>
+      <c r="D2988" t="inlineStr"/>
+      <c r="E2988" t="inlineStr"/>
+      <c r="F2988" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2989">
+      <c r="A2989" t="n">
+        <v>31</v>
+      </c>
+      <c r="B2989" t="inlineStr">
+        <is>
+          <t>[3, 12, 30, 34]</t>
+        </is>
+      </c>
+      <c r="C2989" t="inlineStr"/>
+      <c r="D2989" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2989" t="inlineStr"/>
+      <c r="F2989" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2990">
+      <c r="A2990" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2990" t="inlineStr">
+        <is>
+          <t>[2, 8, 16, 17]</t>
+        </is>
+      </c>
+      <c r="C2990" t="inlineStr"/>
+      <c r="D2990" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2990" t="inlineStr"/>
+      <c r="F2990" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2991">
+      <c r="A2991" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2991" t="inlineStr">
+        <is>
+          <t>[3, 6, 17, 31]</t>
+        </is>
+      </c>
+      <c r="C2991" t="inlineStr"/>
+      <c r="D2991" t="inlineStr"/>
+      <c r="E2991" t="inlineStr"/>
+      <c r="F2991" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2992">
+      <c r="A2992" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2992" t="inlineStr">
+        <is>
+          <t>[6, 7, 16, 31]</t>
+        </is>
+      </c>
+      <c r="C2992" t="inlineStr"/>
+      <c r="D2992" t="inlineStr"/>
+      <c r="E2992" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2992" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2993">
+      <c r="A2993" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2993" t="inlineStr">
+        <is>
+          <t>[0, 1, 7, 14]</t>
+        </is>
+      </c>
+      <c r="C2993" t="inlineStr"/>
+      <c r="D2993" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2993" t="inlineStr"/>
+      <c r="F2993" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2994">
+      <c r="A2994" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2994" t="inlineStr">
+        <is>
+          <t>[6, 10, 17, 18]</t>
+        </is>
+      </c>
+      <c r="C2994" t="inlineStr"/>
+      <c r="D2994" t="inlineStr"/>
+      <c r="E2994" t="inlineStr"/>
+      <c r="F2994" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2995">
+      <c r="A2995" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2995" t="inlineStr">
+        <is>
+          <t>[5, 14, 32, 33]</t>
+        </is>
+      </c>
+      <c r="C2995" t="inlineStr"/>
+      <c r="D2995" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2995" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F2995" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2996">
+      <c r="A2996" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2996" t="inlineStr">
+        <is>
+          <t>[5, 15, 22, 32]</t>
+        </is>
+      </c>
+      <c r="C2996" t="inlineStr"/>
+      <c r="D2996" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2996" t="inlineStr"/>
+      <c r="F2996" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2997">
+      <c r="A2997" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2997" t="inlineStr">
+        <is>
+          <t>[0, 12, 17, 28]</t>
+        </is>
+      </c>
+      <c r="C2997" t="inlineStr"/>
+      <c r="D2997" t="inlineStr"/>
+      <c r="E2997" t="inlineStr"/>
+      <c r="F2997" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2998">
+      <c r="A2998" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2998" t="inlineStr">
+        <is>
+          <t>[3, 30, 32, 34]</t>
+        </is>
+      </c>
+      <c r="C2998" t="inlineStr"/>
+      <c r="D2998" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E2998" t="inlineStr"/>
+      <c r="F2998" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2999">
+      <c r="A2999" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2999" t="inlineStr">
+        <is>
+          <t>[3, 12, 21, 34]</t>
+        </is>
+      </c>
+      <c r="C2999" t="inlineStr"/>
+      <c r="D2999" t="inlineStr"/>
+      <c r="E2999" t="inlineStr"/>
+      <c r="F2999" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3000">
+      <c r="A3000" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3000" t="inlineStr">
+        <is>
+          <t>[10, 11, 12, 34]</t>
+        </is>
+      </c>
+      <c r="C3000" t="inlineStr"/>
+      <c r="D3000" t="inlineStr"/>
+      <c r="E3000" t="inlineStr"/>
+      <c r="F3000" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3001">
+      <c r="A3001" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3001" t="inlineStr">
+        <is>
+          <t>[17, 19, 20, 28]</t>
+        </is>
+      </c>
+      <c r="C3001" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D3001" t="inlineStr"/>
+      <c r="E3001" t="inlineStr"/>
+      <c r="F3001" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3002">
+      <c r="A3002" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3002" t="inlineStr">
+        <is>
+          <t>[0, 8, 17, 35]</t>
+        </is>
+      </c>
+      <c r="C3002" t="inlineStr"/>
+      <c r="D3002" t="inlineStr"/>
+      <c r="E3002" t="inlineStr"/>
+      <c r="F3002" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3003">
+      <c r="A3003" t="n">
+        <v>9</v>
+      </c>
+      <c r="B3003" t="inlineStr">
+        <is>
+          <t>[11, 18, 31, 36]</t>
+        </is>
+      </c>
+      <c r="C3003" t="inlineStr"/>
+      <c r="D3003" t="inlineStr"/>
+      <c r="E3003" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3003" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3004">
+      <c r="A3004" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3004" t="inlineStr">
+        <is>
+          <t>[6, 29, 30, 35]</t>
+        </is>
+      </c>
+      <c r="C3004" t="inlineStr"/>
+      <c r="D3004" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3004" t="inlineStr"/>
+      <c r="F3004" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3005">
+      <c r="A3005" t="n">
+        <v>12</v>
+      </c>
+      <c r="B3005" t="inlineStr">
+        <is>
+          <t>[9, 12, 15, 32]</t>
+        </is>
+      </c>
+      <c r="C3005" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D3005" t="inlineStr"/>
+      <c r="E3005" t="inlineStr"/>
+      <c r="F3005" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3006">
+      <c r="A3006" t="n">
+        <v>12</v>
+      </c>
+      <c r="B3006" t="inlineStr">
+        <is>
+          <t>[12, 15, 25, 32]</t>
+        </is>
+      </c>
+      <c r="C3006" t="inlineStr"/>
+      <c r="D3006" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3006" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3006" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3007">
+      <c r="A3007" t="n">
+        <v>19</v>
+      </c>
+      <c r="B3007" t="inlineStr">
+        <is>
+          <t>[9, 12, 27, 32]</t>
+        </is>
+      </c>
+      <c r="C3007" t="inlineStr"/>
+      <c r="D3007" t="inlineStr"/>
+      <c r="E3007" t="inlineStr"/>
+      <c r="F3007" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3008">
+      <c r="A3008" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3008" t="inlineStr">
+        <is>
+          <t>[9, 12, 18, 35]</t>
+        </is>
+      </c>
+      <c r="C3008" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D3008" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3008" t="inlineStr"/>
+      <c r="F3008" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3009">
+      <c r="A3009" t="n">
+        <v>35</v>
+      </c>
+      <c r="B3009" t="inlineStr">
+        <is>
+          <t>[6, 11, 14, 28]</t>
+        </is>
+      </c>
+      <c r="C3009" t="inlineStr"/>
+      <c r="D3009" t="inlineStr"/>
+      <c r="E3009" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3009" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3010">
+      <c r="A3010" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3010" t="inlineStr">
+        <is>
+          <t>[7, 23, 24, 30]</t>
+        </is>
+      </c>
+      <c r="C3010" t="inlineStr"/>
+      <c r="D3010" t="inlineStr"/>
+      <c r="E3010" t="inlineStr"/>
+      <c r="F3010" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3011">
+      <c r="A3011" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3011" t="inlineStr">
+        <is>
+          <t>[2, 7, 28, 30]</t>
+        </is>
+      </c>
+      <c r="C3011" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D3011" t="inlineStr"/>
+      <c r="E3011" t="inlineStr"/>
+      <c r="F3011" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3012">
+      <c r="A3012" t="n">
+        <v>30</v>
+      </c>
+      <c r="B3012" t="inlineStr">
+        <is>
+          <t>[2, 5, 25, 36]</t>
+        </is>
+      </c>
+      <c r="C3012" t="inlineStr"/>
+      <c r="D3012" t="inlineStr"/>
+      <c r="E3012" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3012" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3013">
+      <c r="A3013" t="n">
+        <v>16</v>
+      </c>
+      <c r="B3013" t="inlineStr">
+        <is>
+          <t>[3, 8, 17, 34]</t>
+        </is>
+      </c>
+      <c r="C3013" t="inlineStr"/>
+      <c r="D3013" t="inlineStr"/>
+      <c r="E3013" t="inlineStr"/>
+      <c r="F3013" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3014">
+      <c r="A3014" t="n">
+        <v>13</v>
+      </c>
+      <c r="B3014" t="inlineStr">
+        <is>
+          <t>[0, 3, 6, 29]</t>
+        </is>
+      </c>
+      <c r="C3014" t="inlineStr"/>
+      <c r="D3014" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3014" t="inlineStr"/>
+      <c r="F3014" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3015">
+      <c r="A3015" t="n">
+        <v>26</v>
+      </c>
+      <c r="B3015" t="inlineStr">
+        <is>
+          <t>[3, 6, 7, 24]</t>
+        </is>
+      </c>
+      <c r="C3015" t="inlineStr"/>
+      <c r="D3015" t="inlineStr"/>
+      <c r="E3015" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3015" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3016">
+      <c r="A3016" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3016" t="inlineStr">
+        <is>
+          <t>[3, 12, 26, 33]</t>
+        </is>
+      </c>
+      <c r="C3016" t="inlineStr"/>
+      <c r="D3016" t="inlineStr"/>
+      <c r="E3016" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3016" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3017">
+      <c r="A3017" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3017" t="inlineStr">
+        <is>
+          <t>[8, 11, 20, 26]</t>
+        </is>
+      </c>
+      <c r="C3017" t="inlineStr"/>
+      <c r="D3017" t="inlineStr"/>
+      <c r="E3017" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3017" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3018">
+      <c r="A3018" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3018" t="inlineStr">
+        <is>
+          <t>[5, 20, 27, 30]</t>
+        </is>
+      </c>
+      <c r="C3018" t="inlineStr"/>
+      <c r="D3018" t="inlineStr"/>
+      <c r="E3018" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3018" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3019">
+      <c r="A3019" t="n">
+        <v>34</v>
+      </c>
+      <c r="B3019" t="inlineStr">
+        <is>
+          <t>[1, 8, 9, 30]</t>
+        </is>
+      </c>
+      <c r="C3019" t="inlineStr"/>
+      <c r="D3019" t="inlineStr"/>
+      <c r="E3019" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3019" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3020">
+      <c r="A3020" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3020" t="inlineStr">
+        <is>
+          <t>[2, 3, 9, 34]</t>
+        </is>
+      </c>
+      <c r="C3020" t="inlineStr"/>
+      <c r="D3020" t="inlineStr"/>
+      <c r="E3020" t="inlineStr"/>
+      <c r="F3020" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3021">
+      <c r="A3021" t="n">
+        <v>16</v>
+      </c>
+      <c r="B3021" t="inlineStr">
+        <is>
+          <t>[12, 21, 30, 34]</t>
+        </is>
+      </c>
+      <c r="C3021" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D3021" t="inlineStr"/>
+      <c r="E3021" t="inlineStr"/>
+      <c r="F3021" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3022">
+      <c r="A3022" t="n">
+        <v>34</v>
+      </c>
+      <c r="B3022" t="inlineStr">
+        <is>
+          <t>[9, 29, 33, 36]</t>
+        </is>
+      </c>
+      <c r="C3022" t="inlineStr"/>
+      <c r="D3022" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3022" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3022" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3023">
+      <c r="A3023" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3023" t="inlineStr">
+        <is>
+          <t>[23, 25, 28, 29]</t>
+        </is>
+      </c>
+      <c r="C3023" t="inlineStr"/>
+      <c r="D3023" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3023" t="inlineStr"/>
+      <c r="F3023" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3024">
+      <c r="A3024" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3024" t="inlineStr">
+        <is>
+          <t>[3, 12, 26, 29]</t>
+        </is>
+      </c>
+      <c r="C3024" t="inlineStr"/>
+      <c r="D3024" t="inlineStr"/>
+      <c r="E3024" t="inlineStr"/>
+      <c r="F3024" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3025">
+      <c r="A3025" t="n">
+        <v>30</v>
+      </c>
+      <c r="B3025" t="inlineStr">
+        <is>
+          <t>[2, 3, 26, 29]</t>
+        </is>
+      </c>
+      <c r="C3025" t="inlineStr"/>
+      <c r="D3025" t="inlineStr"/>
+      <c r="E3025" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3025" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3026">
+      <c r="A3026" t="n">
+        <v>12</v>
+      </c>
+      <c r="B3026" t="inlineStr">
+        <is>
+          <t>[10, 12, 26, 29]</t>
+        </is>
+      </c>
+      <c r="C3026" t="inlineStr"/>
+      <c r="D3026" t="inlineStr"/>
+      <c r="E3026" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3026" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3027">
+      <c r="A3027" t="n">
+        <v>24</v>
+      </c>
+      <c r="B3027" t="inlineStr">
+        <is>
+          <t>[1, 3, 20, 27]</t>
+        </is>
+      </c>
+      <c r="C3027" t="inlineStr"/>
+      <c r="D3027" t="inlineStr"/>
+      <c r="E3027" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3027" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3028">
+      <c r="A3028" t="n">
+        <v>36</v>
+      </c>
+      <c r="B3028" t="inlineStr">
+        <is>
+          <t>[0, 6, 7, 22]</t>
+        </is>
+      </c>
+      <c r="C3028" t="inlineStr"/>
+      <c r="D3028" t="inlineStr"/>
+      <c r="E3028" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3028" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3029">
+      <c r="A3029" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3029" t="inlineStr">
+        <is>
+          <t>[6, 8, 17, 35]</t>
+        </is>
+      </c>
+      <c r="C3029" t="inlineStr"/>
+      <c r="D3029" t="inlineStr"/>
+      <c r="E3029" t="inlineStr"/>
+      <c r="F3029" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3030">
+      <c r="A3030" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3030" t="inlineStr">
+        <is>
+          <t>[1, 10, 26, 29]</t>
+        </is>
+      </c>
+      <c r="C3030" t="inlineStr"/>
+      <c r="D3030" t="inlineStr"/>
+      <c r="E3030" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3030" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3031">
+      <c r="A3031" t="n">
+        <v>32</v>
+      </c>
+      <c r="B3031" t="inlineStr">
+        <is>
+          <t>[2, 13, 26, 29]</t>
+        </is>
+      </c>
+      <c r="C3031" t="inlineStr"/>
+      <c r="D3031" t="inlineStr"/>
+      <c r="E3031" t="inlineStr"/>
+      <c r="F3031" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3032">
+      <c r="A3032" t="n">
+        <v>9</v>
+      </c>
+      <c r="B3032" t="inlineStr">
+        <is>
+          <t>[1, 12, 21, 33]</t>
+        </is>
+      </c>
+      <c r="C3032" t="inlineStr"/>
+      <c r="D3032" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3032" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3032" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3033">
+      <c r="A3033" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3033" t="inlineStr">
+        <is>
+          <t>[1, 22, 23, 27]</t>
+        </is>
+      </c>
+      <c r="C3033" t="inlineStr"/>
+      <c r="D3033" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3033" t="inlineStr"/>
+      <c r="F3033" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3034">
+      <c r="A3034" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3034" t="inlineStr">
+        <is>
+          <t>[0, 6, 27, 28]</t>
+        </is>
+      </c>
+      <c r="C3034" t="inlineStr"/>
+      <c r="D3034" t="inlineStr"/>
+      <c r="E3034" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3034" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3035">
+      <c r="A3035" t="n">
+        <v>35</v>
+      </c>
+      <c r="B3035" t="inlineStr">
+        <is>
+          <t>[6, 8, 17, 32]</t>
+        </is>
+      </c>
+      <c r="C3035" t="inlineStr">
+        <is>
+          <t>acierto</t>
+        </is>
+      </c>
+      <c r="D3035" t="inlineStr"/>
+      <c r="E3035" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3035" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3036">
+      <c r="A3036" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3036" t="inlineStr">
+        <is>
+          <t>[3, 15, 29, 31]</t>
+        </is>
+      </c>
+      <c r="C3036" t="inlineStr"/>
+      <c r="D3036" t="inlineStr"/>
+      <c r="E3036" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3036" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3037">
+      <c r="A3037" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3037" t="inlineStr">
+        <is>
+          <t>[0, 6, 7, 14]</t>
+        </is>
+      </c>
+      <c r="C3037" t="inlineStr"/>
+      <c r="D3037" t="inlineStr"/>
+      <c r="E3037" t="inlineStr"/>
+      <c r="F3037" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3038">
+      <c r="A3038" t="n">
+        <v>33</v>
+      </c>
+      <c r="B3038" t="inlineStr">
+        <is>
+          <t>[7, 19, 32, 35]</t>
+        </is>
+      </c>
+      <c r="C3038" t="inlineStr"/>
+      <c r="D3038" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3038" t="inlineStr"/>
+      <c r="F3038" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3039">
+      <c r="A3039" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3039" t="inlineStr">
+        <is>
+          <t>[6, 16, 22, 23]</t>
+        </is>
+      </c>
+      <c r="C3039" t="inlineStr"/>
+      <c r="D3039" t="inlineStr"/>
+      <c r="E3039" t="inlineStr"/>
+      <c r="F3039" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3040">
+      <c r="A3040" t="n">
+        <v>21</v>
+      </c>
+      <c r="B3040" t="inlineStr">
+        <is>
+          <t>[3, 21, 26, 33]</t>
+        </is>
+      </c>
+      <c r="C3040" t="inlineStr"/>
+      <c r="D3040" t="inlineStr"/>
+      <c r="E3040" t="inlineStr"/>
+      <c r="F3040" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3041">
+      <c r="A3041" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3041" t="inlineStr">
+        <is>
+          <t>[3, 10, 21, 29]</t>
+        </is>
+      </c>
+      <c r="C3041" t="inlineStr"/>
+      <c r="D3041" t="inlineStr"/>
+      <c r="E3041" t="inlineStr"/>
+      <c r="F3041" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3042">
+      <c r="A3042" t="n">
+        <v>27</v>
+      </c>
+      <c r="B3042" t="inlineStr">
+        <is>
+          <t>[1, 17, 20, 33]</t>
+        </is>
+      </c>
+      <c r="C3042" t="inlineStr"/>
+      <c r="D3042" t="inlineStr"/>
+      <c r="E3042" t="inlineStr"/>
+      <c r="F3042" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3043">
+      <c r="A3043" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3043" t="inlineStr">
+        <is>
+          <t>[0, 13, 19, 28]</t>
+        </is>
+      </c>
+      <c r="C3043" t="inlineStr"/>
+      <c r="D3043" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="E3043" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
+      <c r="F3043" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3044">
+      <c r="A3044" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3044" t="inlineStr">
+        <is>
+          <t>[3, 5, 30, 32]</t>
+        </is>
+      </c>
+      <c r="C3044" t="inlineStr"/>
+      <c r="D3044" t="inlineStr"/>
+      <c r="E3044" t="inlineStr"/>
+      <c r="F3044" t="n">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>